<commit_message>
empty id also be ignored
</commit_message>
<xml_diff>
--- a/excels/vertical_types.xlsx
+++ b/excels/vertical_types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3280" windowWidth="27320" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="5860" yWindow="3220" windowWidth="27320" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Vertical" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>FloatTest</t>
   </si>
   <si>
-    <t>BoolTest</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -77,14 +74,47 @@
     <t>2.6</t>
   </si>
   <si>
-    <t>随便写一些东西作为注释，这些不会被导出</t>
+    <t>BoolTest2</t>
+  </si>
+  <si>
+    <t>BoolTest1</t>
+  </si>
+  <si>
+    <t>BoolTest3</t>
+  </si>
+  <si>
+    <t>BoolTest4</t>
+  </si>
+  <si>
+    <t>BoolTest5</t>
+  </si>
+  <si>
+    <t>BoolTest6</t>
+  </si>
+  <si>
+    <t>BoolTest7</t>
+  </si>
+  <si>
+    <t>BoolTest8</t>
+  </si>
+  <si>
+    <t>BoolTest9</t>
+  </si>
+  <si>
+    <t>BoolTest10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <t xml:space="preserve">false  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +125,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,14 +163,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,90 +459,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E1" sqref="E1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1">
         <v>1001</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>345</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>